<commit_message>
update function to add row color based on value.
</commit_message>
<xml_diff>
--- a/Utilities/Txt2Xls/outtest.xlsx
+++ b/Utilities/Txt2Xls/outtest.xlsx
@@ -14,16 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>a</t>
   </si>
@@ -44,6 +35,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>x1</t>
   </si>
 </sst>
 </file>
@@ -59,12 +53,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -79,21 +79,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -383,57 +377,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1">
         <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A4:E4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
-      <formula>B4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
-      <formula>B4</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>